<commit_message>
fixed BT rotation bug
로테이션 값에 로테이션 스피드가 아니라 무프 스피드가 들어가서 생기는 버그를 해결했다.
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB49F71-BB34-4B5B-BD7E-4B73F001A382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB83126-5594-48CA-A9D3-85871C57B210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-4065" windowWidth="29040" windowHeight="15840" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
@@ -508,7 +508,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -615,7 +615,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>2.5</v>
@@ -636,7 +636,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="K3" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
add SliderUI, phero bar UI, apply layer to Canvas in UIs
캔버스 픽셀 쉐이더에서 UV값의 U에 따라 값을 비교해서 0에서 1로 정규화된 상수 버퍼 값보다 UV의 U 값이 큰 경우 discard를 통해서 슬라이더 효과를 낼 수 있는 SliderUI를 구현하였다.
현재 보유 중인 페로 양에 따라 변하는 UI 페로 바를 구현하였다.
페로를 획득했을 때와 페로를 사용했을 때 보간을 통해 자연스럽게 변할 수 있도록 구현하였다.
캔버스가 들고 있는 UI들을 배열을 통해서 레이어를 나눠 그리는 순서를 정하도록 구현하였다.
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB83126-5594-48CA-A9D3-85871C57B210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1AAA33-A7CF-4F68-A9FF-8693A02A23B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-4065" windowWidth="29040" windowHeight="15840" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
@@ -508,7 +508,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -595,7 +595,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="K2" t="s">
         <v>11</v>
@@ -615,7 +615,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>2.5</v>
@@ -636,7 +636,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="K3" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
apply phero system in ShieldAbility
임시적으로 쉴드 어빌리티에 페로 시스템을 추가하여 쉴드 사용 시 보유중인 페로를 소비하도록 구현하였다.
보유중인 페로가 부족할 경우 실행하지 않는다.
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1AAA33-A7CF-4F68-A9FF-8693A02A23B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E899DA7E-757B-49A2-AE07-123D59DBD9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-4065" windowWidth="29040" windowHeight="15840" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
+    <workbookView xWindow="4830" yWindow="4905" windowWidth="28800" windowHeight="15435" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -508,7 +508,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -595,7 +595,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="K2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
add make an attack between enemies, add AI AttackRotationSpeed
페로 특수 능력 마인드 컨트롤을 구현하기 위해 적끼리 공격할 수 있도록 타겟을 플레이어 뿐만 아니라 적 AI끼리도 상호작용할 수 있도록 변경했다. 이 과정에서 순환참조 문제를 해결하기 위해 타겟을 생포인터로 변경하였다.
추가로 적 공격 중 플레이어 쪽을 향하여 돌게 함으로써 플레이어 주변을 도는 문제를 해결하였다.
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E899DA7E-757B-49A2-AE07-123D59DBD9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9901EB1-19FF-4EB2-9D18-F14A25B81191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="4905" windowWidth="28800" windowHeight="15435" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
+    <workbookView xWindow="38280" yWindow="-4065" windowWidth="29040" windowHeight="15840" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Ursacetus</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -121,6 +121,10 @@
   </si>
   <si>
     <t>MaxHp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackRotationSpeed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -505,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CEE82F-9CE1-43EA-80A5-B7D491C6FD38}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -517,18 +521,19 @@
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -539,34 +544,37 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -580,34 +588,37 @@
         <v>2.5</v>
       </c>
       <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
         <v>150</v>
       </c>
-      <c r="F2">
-        <v>15</v>
-      </c>
       <c r="G2">
+        <v>250</v>
+      </c>
+      <c r="H2">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>4</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>70</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -621,34 +632,37 @@
         <v>2.5</v>
       </c>
       <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
         <v>150</v>
       </c>
-      <c r="F3">
+      <c r="G3">
+        <v>250</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1.5</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>150</v>
+      </c>
+      <c r="L3" t="s">
         <v>15</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1.5</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>150</v>
-      </c>
-      <c r="K3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>14</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -662,30 +676,33 @@
         <v>3.5</v>
       </c>
       <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
         <v>150</v>
       </c>
-      <c r="F4">
-        <v>20</v>
-      </c>
       <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>7.5</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1000</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>18</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>17</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change SliderBarUI from script to normal class, add HpBarUI, hit player
슬라이더 바를 페로뿐만 아니라 HP에서도 사용하기 위해서 스크립트가 아닌 UI 묶음을 담는 SliderBarUI 클래스를 구현하였다. 그리고 페로 플레이어는 해당 클래스를 내부적으로 가지고 있기로 변경하였다. 이렇게 해야 슬라이더 바에 대한 관리가 쉽기 때문이다.
구현한 슬라이더바 UI 클래스를 사용해 추가적으로 HP 바를 구현하였으며 플레이어가 보스의 공격에 맞으면 HP가 줄도록 구현하였다. HP가 0이 되면 스폰 지점에서 리스폰된다.
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9901EB1-19FF-4EB2-9D18-F14A25B81191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473EE582-6CB1-4C72-A819-BA95AE7A413E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-4065" windowWidth="29040" windowHeight="15840" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
@@ -512,7 +512,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -597,7 +597,7 @@
         <v>250</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -641,7 +641,7 @@
         <v>250</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I3">
         <v>1.5</v>
@@ -685,7 +685,7 @@
         <v>10</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I4">
         <v>7.5</v>

</xml_diff>

<commit_message>
add mind control aim UI, apply enemy attack each other
마인드 컨트롤 에임 UI를 구현하였으며 사용하기 편하게 UI에서 Texture, width, height를 묶어서 사용할 수 있도록 UITexture를 구현하였다.  UITexture는 sptr이 아닌 일반 변수로 가지고 있어도 될 것 같다.
추가로 적의 공격에 플레이어가 데미지를 받거나 적 끼리 공격하여 데미지를 적용할 수 있도록 적 공격 구현을 완료하였다.
마인드 컨트롤 된 적에게 쉴드 100을 추가하도록 하였다.
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473EE582-6CB1-4C72-A819-BA95AE7A413E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87873AE9-54D2-4AB3-92AB-4EC075323023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-4065" windowWidth="29040" windowHeight="15840" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
@@ -512,7 +512,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
complete stage1 boss attack pattern, add attack indicator
스테이지 1의 보스 공격 패턴과 공격 표시를 추가하였다. 추후에 보스 공격시 파티클을 추가해야 한다.
공격은 애니메이션 파라미터의 정수값으로 기본, 스킬 공격을 정하게 되고 스킬 사용 때가 되면 미리 넣어둔 어빌리티를 작동시킨다.
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13682CB2-A834-4D0A-B42F-8361057003A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45639C27-C798-42C7-ADBD-D7C4732AF7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="11370" windowWidth="28800" windowHeight="15435" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
+    <workbookView xWindow="38280" yWindow="-4065" windowWidth="29040" windowHeight="15840" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>Ursacetus</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,10 +65,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AttackAnimName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GetHitAnimName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -104,10 +100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2HandsSmashAttack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PheroLevel</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -205,6 +197,34 @@
   </si>
   <si>
     <t>DodgeForward</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LeftHandAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack2AnimName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LeftFootStompAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Roar1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack3AnimName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack1AnimName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -589,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CEE82F-9CE1-43EA-80A5-B7D491C6FD38}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -609,17 +629,17 @@
     <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="28" customWidth="1"/>
-    <col min="13" max="13" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.375" customWidth="1"/>
     <col min="14" max="14" width="18.625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -631,7 +651,7 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -643,19 +663,25 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -687,21 +713,27 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -731,21 +763,27 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M3" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="N3" t="s">
-        <v>13</v>
+        <v>44</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -778,18 +816,24 @@
         <v>200</v>
       </c>
       <c r="L4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M4" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="N4" t="s">
-        <v>13</v>
+        <v>44</v>
+      </c>
+      <c r="O4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -822,18 +866,24 @@
         <v>150</v>
       </c>
       <c r="L5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" t="s">
         <v>15</v>
       </c>
-      <c r="M5" t="s">
-        <v>14</v>
-      </c>
-      <c r="N5" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -863,19 +913,25 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M6" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="N6" t="s">
-        <v>13</v>
+        <v>44</v>
+      </c>
+      <c r="O6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -886,7 +942,7 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -901,7 +957,7 @@
         <v>200</v>
       </c>
       <c r="I7">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -910,18 +966,24 @@
         <v>1000</v>
       </c>
       <c r="L7" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="M7" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="N7" t="s">
-        <v>13</v>
+        <v>45</v>
+      </c>
+      <c r="O7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -954,83 +1016,95 @@
         <v>200</v>
       </c>
       <c r="L8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M8" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="N8" t="s">
-        <v>13</v>
+        <v>44</v>
+      </c>
+      <c r="O8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P8" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F9">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="G9">
+        <v>250</v>
+      </c>
+      <c r="H9">
         <v>100</v>
       </c>
-      <c r="H9">
-        <v>300</v>
-      </c>
       <c r="I9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="L9" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="M9" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="N9" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="O9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P9" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="E10">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F10">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="G10">
         <v>250</v>
       </c>
       <c r="H10">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -1039,65 +1113,77 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="L10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M10" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="N10" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="O10" t="s">
+        <v>16</v>
+      </c>
+      <c r="P10" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>6</v>
       </c>
       <c r="D11">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="E11">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F11">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="G11">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="H11">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="L11" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M11" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="N11" t="s">
-        <v>13</v>
+        <v>44</v>
+      </c>
+      <c r="O11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>8</v>
@@ -1130,18 +1216,24 @@
         <v>600</v>
       </c>
       <c r="L12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N12" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="O12" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N9">
-    <sortCondition ref="B2:B9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P12">
+    <sortCondition ref="B2:B12"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[JJM] Update Network Structure, Update Bullet Send OnShoot
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13682CB2-A834-4D0A-B42F-8361057003A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF3FF4E-FEE6-4E99-85C0-433E1F685AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="11370" windowWidth="28800" windowHeight="15435" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
+    <workbookView xWindow="39180" yWindow="-3165" windowWidth="21600" windowHeight="11385" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -901,7 +901,7 @@
         <v>200</v>
       </c>
       <c r="I7">
-        <v>7.5</v>
+        <v>4.5</v>
       </c>
       <c r="J7">
         <v>0</v>

</xml_diff>

<commit_message>
change stage2 boss attack animation
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45639C27-C798-42C7-ADBD-D7C4732AF7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E68252-0861-4C64-85EB-0E3D9E779FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-4065" windowWidth="29040" windowHeight="15840" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
+    <workbookView xWindow="38415" yWindow="-3900" windowWidth="30210" windowHeight="17340" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
   <si>
     <t>Ursacetus</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -148,10 +148,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Direct2HitComboAttackForward</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Blocked</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -225,6 +221,18 @@
   </si>
   <si>
     <t>Attack1AnimName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UppercutDiggerAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UppercutDrillAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SmashAttack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -612,7 +620,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -666,13 +674,13 @@
         <v>19</v>
       </c>
       <c r="L1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O1" t="s">
         <v>8</v>
@@ -719,10 +727,10 @@
         <v>10</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O2" t="s">
         <v>11</v>
@@ -769,10 +777,10 @@
         <v>22</v>
       </c>
       <c r="M3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O3" t="s">
         <v>16</v>
@@ -783,7 +791,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -819,13 +827,13 @@
         <v>16</v>
       </c>
       <c r="M4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P4" t="s">
         <v>12</v>
@@ -869,10 +877,10 @@
         <v>14</v>
       </c>
       <c r="M5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O5" t="s">
         <v>13</v>
@@ -919,10 +927,10 @@
         <v>24</v>
       </c>
       <c r="M6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O6" t="s">
         <v>16</v>
@@ -966,16 +974,16 @@
         <v>1000</v>
       </c>
       <c r="L7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P7" t="s">
         <v>12</v>
@@ -1019,10 +1027,10 @@
         <v>26</v>
       </c>
       <c r="M8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O8" t="s">
         <v>16</v>
@@ -1033,7 +1041,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -1066,24 +1074,24 @@
         <v>500</v>
       </c>
       <c r="L9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O9" t="s">
         <v>16</v>
       </c>
       <c r="P9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -1116,13 +1124,13 @@
         <v>300</v>
       </c>
       <c r="L10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O10" t="s">
         <v>16</v>
@@ -1151,7 +1159,7 @@
         <v>150</v>
       </c>
       <c r="G11">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="H11">
         <v>300</v>
@@ -1166,24 +1174,24 @@
         <v>1500</v>
       </c>
       <c r="L11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" t="s">
         <v>29</v>
       </c>
-      <c r="M11" t="s">
-        <v>44</v>
-      </c>
-      <c r="N11" t="s">
-        <v>44</v>
-      </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>30</v>
-      </c>
-      <c r="P11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>8</v>
@@ -1216,19 +1224,19 @@
         <v>600</v>
       </c>
       <c r="L12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
apply remote player death async
리모트 플레이어의 죽음 동기화 완료
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alseh\Desktop\X-MACHINA\Client\X-MACHINA\Import\XL\Enemy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6145D5-A5DA-4D02-ACEF-75944C660DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A823B15D-6DF3-456E-9F89-1C9232609141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
+    <workbookView xWindow="5475" yWindow="13620" windowWidth="30210" windowHeight="17340" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -620,7 +620,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
complete stage1 boss attack sync
보스 공격 동기화를 완료 했으나 블랜딩 문제는 추후 해결
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154EF463-E089-43E7-B049-6CEF4ED73120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D813E93C-C07F-4E73-A727-6A815DC7A0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-4065" windowWidth="29040" windowHeight="15840" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -620,7 +620,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -706,7 +706,7 @@
         <v>15</v>
       </c>
       <c r="F2">
-        <v>150</v>
+        <v>500</v>
       </c>
       <c r="G2">
         <v>250</v>
@@ -756,7 +756,7 @@
         <v>10</v>
       </c>
       <c r="F3">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="G3">
         <v>250</v>
@@ -806,7 +806,7 @@
         <v>20</v>
       </c>
       <c r="F4">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="G4">
         <v>250</v>
@@ -856,7 +856,7 @@
         <v>15</v>
       </c>
       <c r="F5">
-        <v>150</v>
+        <v>500</v>
       </c>
       <c r="G5">
         <v>250</v>
@@ -906,7 +906,7 @@
         <v>10</v>
       </c>
       <c r="F6">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="G6">
         <v>250</v>
@@ -956,7 +956,7 @@
         <v>20</v>
       </c>
       <c r="F7">
-        <v>150</v>
+        <v>500</v>
       </c>
       <c r="G7">
         <v>10</v>
@@ -1006,7 +1006,7 @@
         <v>10</v>
       </c>
       <c r="F8">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="G8">
         <v>250</v>
@@ -1056,7 +1056,7 @@
         <v>25</v>
       </c>
       <c r="F9">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="G9">
         <v>250</v>
@@ -1106,7 +1106,7 @@
         <v>30</v>
       </c>
       <c r="F10">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="G10">
         <v>250</v>
@@ -1156,7 +1156,7 @@
         <v>20</v>
       </c>
       <c r="F11">
-        <v>150</v>
+        <v>500</v>
       </c>
       <c r="G11">
         <v>100</v>
@@ -1206,7 +1206,7 @@
         <v>20</v>
       </c>
       <c r="F12">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="G12">
         <v>250</v>

</xml_diff>

<commit_message>
complete mind control sync
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D813E93C-C07F-4E73-A727-6A815DC7A0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36C3026-78BB-431F-937F-0B83A56D6732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
+    <workbookView xWindow="12480" yWindow="3390" windowWidth="22665" windowHeight="12885" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CEE82F-9CE1-43EA-80A5-B7D491C6FD38}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -933,7 +933,7 @@
         <v>43</v>
       </c>
       <c r="O6" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="P6" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
update deus phase 1
</commit_message>
<xml_diff>
--- a/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
+++ b/Client/X-MACHINA/Import/XL/Enemy/EnemyStat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\DirectX12_Project\Client\X-MACHINA\Import\XL\Enemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36C3026-78BB-431F-937F-0B83A56D6732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CD75DD-DE8C-434F-A1CB-D7EDB446F900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12480" yWindow="3390" windowWidth="22665" windowHeight="12885" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
+    <workbookView xWindow="38280" yWindow="-4065" windowWidth="29040" windowHeight="15840" xr2:uid="{06281053-F3D5-4E77-9DAD-CE711606AC4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
   <si>
     <t>Ursacetus</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -233,6 +233,34 @@
   </si>
   <si>
     <t>SmashAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deus_Phase_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deus_Phase_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attack_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shot_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shot_02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Get_Hit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dead_02</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -617,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CEE82F-9CE1-43EA-80A5-B7D491C6FD38}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1239,6 +1267,106 @@
         <v>30</v>
       </c>
     </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>500</v>
+      </c>
+      <c r="G13">
+        <v>250</v>
+      </c>
+      <c r="H13">
+        <v>300</v>
+      </c>
+      <c r="I13">
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>3000</v>
+      </c>
+      <c r="L13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" t="s">
+        <v>54</v>
+      </c>
+      <c r="N13" t="s">
+        <v>55</v>
+      </c>
+      <c r="O13" t="s">
+        <v>56</v>
+      </c>
+      <c r="P13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="F14">
+        <v>500</v>
+      </c>
+      <c r="G14">
+        <v>250</v>
+      </c>
+      <c r="H14">
+        <v>300</v>
+      </c>
+      <c r="I14">
+        <v>7</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>3000</v>
+      </c>
+      <c r="L14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P12">
     <sortCondition ref="B2:B12"/>

</xml_diff>